<commit_message>
Ajustando as bases para analise
</commit_message>
<xml_diff>
--- a/produtos_data.xlsx
+++ b/produtos_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wende\Desktop\dados2.0\Projetos\Analise_Vendas_e_Performance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wendell Barcelos\Desktop\Dados\Projeto\Análise de Vendas e Performance de Produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03CCCD97-E575-46A7-9565-59BFC8713413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20778CFD-4B45-4C5F-A6C9-3FB635B92737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="255" windowWidth="14880" windowHeight="14265" xr2:uid="{9B050460-54EF-4F16-91C4-1C3259DE965E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9B050460-54EF-4F16-91C4-1C3259DE965E}"/>
   </bookViews>
   <sheets>
     <sheet name="produto_data" sheetId="1" r:id="rId1"/>
@@ -40,382 +40,382 @@
     <t>QtdEstoque</t>
   </si>
   <si>
-    <t>05112d7f-12ec-4f24-8bab-4c1b904aa134</t>
-  </si>
-  <si>
     <t>Teclado Mecânico</t>
   </si>
   <si>
     <t>Acessórios Informática</t>
   </si>
   <si>
-    <t>79f73374-e92a-409b-92f1-8f28a61bdc7d</t>
-  </si>
-  <si>
     <t>Mouse Sem Fio</t>
   </si>
   <si>
-    <t>62d47bff-a510-47b4-924d-4a86efed0e52</t>
-  </si>
-  <si>
     <t>Mouse Gamer</t>
   </si>
   <si>
-    <t>63032bd4-9db5-44b5-af84-22cc484fda28</t>
-  </si>
-  <si>
     <t>Headset Gamer</t>
   </si>
   <si>
-    <t>3cd7e0ea-bf81-4a17-a905-8f29731da6ec</t>
-  </si>
-  <si>
     <t>Hub USB</t>
   </si>
   <si>
-    <t>4002c5eb-9cd3-4931-bd95-7e47aed14cec</t>
-  </si>
-  <si>
     <t>Cabo HDMI</t>
   </si>
   <si>
-    <t>a2fe9cb4-fcec-4791-bae9-df3f585b8128</t>
-  </si>
-  <si>
     <t>Cadeira Gamer</t>
   </si>
   <si>
-    <t>e6092042-eb5f-4944-baa8-34197479d994</t>
-  </si>
-  <si>
     <t>Monitor Suporte</t>
   </si>
   <si>
-    <t>e123433f-8955-47ec-b447-f8a127340be8</t>
-  </si>
-  <si>
     <t>Base para Notebook</t>
   </si>
   <si>
-    <t>496fe308-24f7-4239-b94d-91565c31d125</t>
-  </si>
-  <si>
     <t>Adaptador USB</t>
   </si>
   <si>
-    <t>f689c4c2-2ca2-4887-bb21-68c4a3188a65</t>
-  </si>
-  <si>
     <t>Smartwatch</t>
   </si>
   <si>
     <t>Tecnologia</t>
   </si>
   <si>
-    <t>41d893a5-ffc7-4ba2-a371-9357f7a58f8d</t>
-  </si>
-  <si>
     <t>Assistente Virtual</t>
   </si>
   <si>
-    <t>bd71017f-5e3a-4dad-a90a-8303e1c6a7c2</t>
-  </si>
-  <si>
     <t>Carregador Rápido</t>
   </si>
   <si>
-    <t>4cc378c3-ce32-40af-ae86-49f1055c22ad</t>
-  </si>
-  <si>
     <t>Tablet</t>
   </si>
   <si>
-    <t>690e1a7e-75be-4ba7-8ae4-e09624dc1ee5</t>
-  </si>
-  <si>
     <t>HD Externo</t>
   </si>
   <si>
-    <t>da07f08e-8a9f-45a1-a13a-e6f4b5ef818b</t>
-  </si>
-  <si>
     <t>SSD</t>
   </si>
   <si>
-    <t>2001965b-66f8-4b87-bccc-1a7d3a1bba9c</t>
-  </si>
-  <si>
     <t>Power Bank</t>
   </si>
   <si>
-    <t>35461a1c-5a5a-4dac-a062-4c48d7131c2e</t>
-  </si>
-  <si>
     <t>Projetor Portátil</t>
   </si>
   <si>
-    <t>e23509a8-6bcf-4fa4-a7e2-020ef11f1e97</t>
-  </si>
-  <si>
     <t>Drone</t>
   </si>
   <si>
-    <t>73cab4e3-bbc3-453b-b5e8-abfe6af01106</t>
-  </si>
-  <si>
     <t>Echo Dot</t>
   </si>
   <si>
-    <t>76a90f78-6370-4da9-b3ce-caaf71a2f6c1</t>
-  </si>
-  <si>
     <t>Console PS5</t>
   </si>
   <si>
     <t>Games</t>
   </si>
   <si>
-    <t>aa55e9af-5375-44b0-967a-25f85d12490e</t>
-  </si>
-  <si>
     <t>Console Xbox Series X</t>
   </si>
   <si>
-    <t>87a9efaf-b92a-41b7-a213-cdad661d3354</t>
-  </si>
-  <si>
     <t>Joystick para PC</t>
   </si>
   <si>
-    <t>b66c4a03-378a-4526-befa-528c34b6d9da</t>
-  </si>
-  <si>
     <t>Controle Xbox</t>
   </si>
   <si>
-    <t>f2b074a3-31d1-4ea8-9181-c8a230e31645</t>
-  </si>
-  <si>
     <t>Controle DualSense</t>
   </si>
   <si>
-    <t>c8bc7784-a8c9-4656-bab3-d9a3dfa4a6da</t>
-  </si>
-  <si>
     <t>Headset para Xbox</t>
   </si>
   <si>
-    <t>769fce1a-e67d-4f00-9d08-c2549e6eac9c</t>
-  </si>
-  <si>
     <t>Volante para Simulação</t>
   </si>
   <si>
-    <t>cac5a4c6-c393-4806-9cc8-c8018c573243</t>
-  </si>
-  <si>
     <t>Cadeira Gamer RGB</t>
   </si>
   <si>
-    <t>4e90ee87-a4dd-4fe1-9ff3-fbbf6880534f</t>
-  </si>
-  <si>
     <t>Teclado para Consoles</t>
   </si>
   <si>
-    <t>78612769-242e-4cff-a490-7a6336a8d53d</t>
-  </si>
-  <si>
     <t>Dock para Switch</t>
   </si>
   <si>
-    <t>73cb3b3f-a6f9-4864-8af6-d2681bd07f9b</t>
-  </si>
-  <si>
     <t>TV 4K</t>
   </si>
   <si>
     <t>Eletro-Eletrônicos</t>
   </si>
   <si>
-    <t>f4aae84a-d538-4419-a798-d9bf4ce1ca16</t>
-  </si>
-  <si>
     <t>Home Theater</t>
   </si>
   <si>
-    <t>69808e3c-9fa3-4e4b-9ebf-96d3c64ab8bf</t>
-  </si>
-  <si>
     <t>Soundbar</t>
   </si>
   <si>
-    <t>56726735-3798-4c80-b30c-84610d06d891</t>
-  </si>
-  <si>
     <t>Receptor de TV</t>
   </si>
   <si>
-    <t>a8deeb1c-281e-4259-a3d2-1a338d3bc1df</t>
-  </si>
-  <si>
     <t>Rádio Portátil</t>
   </si>
   <si>
-    <t>6e896265-847a-4fa5-afe7-39dd6260dcbe</t>
-  </si>
-  <si>
     <t>Caixa de Som Bluetooth</t>
   </si>
   <si>
-    <t>061a1396-7167-48ee-b175-82082e292386</t>
-  </si>
-  <si>
     <t>Smart TV</t>
   </si>
   <si>
-    <t>9140a95d-62ce-4959-b4da-1f50b1a7fe09</t>
-  </si>
-  <si>
     <t>Controle Remoto Universal</t>
   </si>
   <si>
-    <t>fbcf57d7-45f8-4c5d-ac1e-86bbaac016bd</t>
-  </si>
-  <si>
     <t>Antena Digital</t>
   </si>
   <si>
-    <t>c4ecea32-9038-4f81-ae3d-c742bef8004b</t>
-  </si>
-  <si>
     <t>Carregador Universal</t>
   </si>
   <si>
-    <t>9337bb34-66e1-408e-a428-2ec427e6287b</t>
-  </si>
-  <si>
     <t>iPhone 14</t>
   </si>
   <si>
     <t>Celulares</t>
   </si>
   <si>
-    <t>26932d95-32a3-48fb-8d03-a402c827e7c0</t>
-  </si>
-  <si>
     <t>Samsung Galaxy S23</t>
   </si>
   <si>
-    <t>3ee61872-77f4-47f9-9105-88a9694a48b3</t>
-  </si>
-  <si>
     <t>Moto G Power</t>
   </si>
   <si>
-    <t>c33b14ed-216c-4ed0-bd0c-1656de373877</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi Note 12</t>
   </si>
   <si>
-    <t>9c406cbe-50f3-40af-bc97-6337ee668fd2</t>
-  </si>
-  <si>
     <t>Realme Narzo</t>
   </si>
   <si>
-    <t>87d49f49-9cc1-4301-836d-b2eceeda69bc</t>
-  </si>
-  <si>
     <t>OnePlus Nord</t>
   </si>
   <si>
-    <t>09098704-e03c-419a-a0ca-381cbc3dc68a</t>
-  </si>
-  <si>
     <t>Fone Bluetooth</t>
   </si>
   <si>
-    <t>10bb5ed3-c976-4bdf-98d9-39ebad1abfd5</t>
-  </si>
-  <si>
     <t>Carregador Wireless</t>
   </si>
   <si>
-    <t>eb9060cb-0238-4c49-857e-ccfa15f3b747</t>
-  </si>
-  <si>
     <t>Capa Protetora</t>
   </si>
   <si>
-    <t>54ddbff4-0d81-439d-9e95-2d1ddcbc5e3f</t>
-  </si>
-  <si>
     <t>Película de Vidro</t>
   </si>
   <si>
-    <t>ee7ae3bb-5034-4715-9706-c3cdda440dee</t>
-  </si>
-  <si>
     <t>Geladeira Frost Free</t>
   </si>
   <si>
     <t>Eletro-Domésticos</t>
   </si>
   <si>
-    <t>be5b8a92-33f8-457c-9b50-73c7e6dc9c76</t>
-  </si>
-  <si>
     <t>Máquina de Lavar</t>
   </si>
   <si>
-    <t>4ebc5f60-3687-41e1-b53c-a48b268de9f4</t>
-  </si>
-  <si>
     <t>Forno Microondas</t>
   </si>
   <si>
-    <t>9f8c1c81-5ce9-43d3-90e6-e383d736b50e</t>
-  </si>
-  <si>
     <t>Fogão 4 Bocas</t>
   </si>
   <si>
-    <t>e78e4df0-955c-41d2-90c4-9c2be8c451fc</t>
-  </si>
-  <si>
     <t>Aspirador de Pó</t>
   </si>
   <si>
-    <t>56afd9ce-799f-42c0-b255-7e4ed4087cd1</t>
-  </si>
-  <si>
     <t>Liquidificador</t>
   </si>
   <si>
-    <t>4da12b02-4a2c-4830-acdb-1625b41f5721</t>
-  </si>
-  <si>
     <t>Airfryer</t>
   </si>
   <si>
-    <t>28e9772b-8fd7-4ced-8d65-e32819fbded2</t>
-  </si>
-  <si>
     <t>Cafeteira</t>
   </si>
   <si>
-    <t>29cb31b1-26ea-445e-a16c-77ace69bf25c</t>
-  </si>
-  <si>
     <t>Ventilador</t>
   </si>
   <si>
-    <t>e904ee42-8845-46f5-9e52-1d486a499f0b</t>
-  </si>
-  <si>
     <t>Purificador de Água</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>P008</t>
+  </si>
+  <si>
+    <t>P009</t>
+  </si>
+  <si>
+    <t>P010</t>
+  </si>
+  <si>
+    <t>P011</t>
+  </si>
+  <si>
+    <t>P012</t>
+  </si>
+  <si>
+    <t>P013</t>
+  </si>
+  <si>
+    <t>P014</t>
+  </si>
+  <si>
+    <t>P015</t>
+  </si>
+  <si>
+    <t>P016</t>
+  </si>
+  <si>
+    <t>P017</t>
+  </si>
+  <si>
+    <t>P018</t>
+  </si>
+  <si>
+    <t>P019</t>
+  </si>
+  <si>
+    <t>P020</t>
+  </si>
+  <si>
+    <t>P021</t>
+  </si>
+  <si>
+    <t>P022</t>
+  </si>
+  <si>
+    <t>P023</t>
+  </si>
+  <si>
+    <t>P024</t>
+  </si>
+  <si>
+    <t>P025</t>
+  </si>
+  <si>
+    <t>P026</t>
+  </si>
+  <si>
+    <t>P027</t>
+  </si>
+  <si>
+    <t>P028</t>
+  </si>
+  <si>
+    <t>P029</t>
+  </si>
+  <si>
+    <t>P030</t>
+  </si>
+  <si>
+    <t>P031</t>
+  </si>
+  <si>
+    <t>P032</t>
+  </si>
+  <si>
+    <t>P033</t>
+  </si>
+  <si>
+    <t>P034</t>
+  </si>
+  <si>
+    <t>P035</t>
+  </si>
+  <si>
+    <t>P036</t>
+  </si>
+  <si>
+    <t>P037</t>
+  </si>
+  <si>
+    <t>P038</t>
+  </si>
+  <si>
+    <t>P039</t>
+  </si>
+  <si>
+    <t>P040</t>
+  </si>
+  <si>
+    <t>P041</t>
+  </si>
+  <si>
+    <t>P042</t>
+  </si>
+  <si>
+    <t>P043</t>
+  </si>
+  <si>
+    <t>P044</t>
+  </si>
+  <si>
+    <t>P045</t>
+  </si>
+  <si>
+    <t>P046</t>
+  </si>
+  <si>
+    <t>P047</t>
+  </si>
+  <si>
+    <t>P048</t>
+  </si>
+  <si>
+    <t>P049</t>
+  </si>
+  <si>
+    <t>P050</t>
+  </si>
+  <si>
+    <t>P051</t>
+  </si>
+  <si>
+    <t>P052</t>
+  </si>
+  <si>
+    <t>P053</t>
+  </si>
+  <si>
+    <t>P054</t>
+  </si>
+  <si>
+    <t>P055</t>
+  </si>
+  <si>
+    <t>P056</t>
+  </si>
+  <si>
+    <t>P057</t>
+  </si>
+  <si>
+    <t>P058</t>
+  </si>
+  <si>
+    <t>P059</t>
+  </si>
+  <si>
+    <t>P060</t>
   </si>
 </sst>
 </file>
@@ -899,9 +899,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1259,7 +1258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8128BBA1-BE86-4B40-BFA7-E332AF9A473F}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1285,13 +1286,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>378.58</v>
@@ -1305,13 +1306,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>96.74</v>
@@ -1325,13 +1326,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>400.01</v>
@@ -1345,13 +1346,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>412.87</v>
@@ -1365,13 +1366,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>47.94</v>
@@ -1385,13 +1386,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>21.88</v>
@@ -1405,13 +1406,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>1209.96</v>
@@ -1425,13 +1426,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>999.96</v>
@@ -1445,13 +1446,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>89.72</v>
@@ -1465,13 +1466,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>27.25</v>
@@ -1485,13 +1486,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>96.49</v>
@@ -1505,13 +1506,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>373.17</v>
@@ -1525,13 +1526,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>169.22</v>
@@ -1545,13 +1546,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D15">
         <v>1294.6500000000001</v>
@@ -1565,13 +1566,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>396.38</v>
@@ -1585,13 +1586,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>446.75</v>
@@ -1605,13 +1606,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>65.22</v>
@@ -1625,13 +1626,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>129.47</v>
@@ -1645,13 +1646,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>1393.99</v>
@@ -1665,13 +1666,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D21">
         <v>315.06</v>
@@ -1685,13 +1686,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>4912.2299999999996</v>
@@ -1705,13 +1706,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>1818.61</v>
@@ -1725,13 +1726,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D24">
         <v>478.65</v>
@@ -1745,13 +1746,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D25">
         <v>502.37</v>
@@ -1765,13 +1766,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>456.62</v>
@@ -1785,13 +1786,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D27">
         <v>111.24</v>
@@ -1805,13 +1806,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D28">
         <v>1810.8</v>
@@ -1825,13 +1826,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D29">
         <v>897.12</v>
@@ -1845,13 +1846,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D30">
         <v>193.44</v>
@@ -1865,13 +1866,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D31">
         <v>177.08</v>
@@ -1885,13 +1886,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D32">
         <v>2941.32</v>
@@ -1905,13 +1906,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>438.44</v>
@@ -1925,13 +1926,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>399.89</v>
@@ -1945,13 +1946,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <v>39.9</v>
@@ -1965,13 +1966,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D36">
         <v>60.22</v>
@@ -1984,14 +1985,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>80</v>
+      <c r="A37" t="s">
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D37">
         <v>383.49</v>
@@ -2005,13 +2006,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D38">
         <v>1660.72</v>
@@ -2025,13 +2026,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D39">
         <v>22.16</v>
@@ -2045,13 +2046,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D40">
         <v>61</v>
@@ -2065,13 +2066,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D41">
         <v>83.89</v>
@@ -2085,13 +2086,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D42">
         <v>4033.37</v>
@@ -2105,13 +2106,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D43">
         <v>3451.75</v>
@@ -2125,13 +2126,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D44">
         <v>2562.06</v>
@@ -2145,13 +2146,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D45">
         <v>2074.58</v>
@@ -2165,13 +2166,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D46">
         <v>1344.95</v>
@@ -2185,13 +2186,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D47">
         <v>4054.7</v>
@@ -2205,13 +2206,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D48">
         <v>126.23</v>
@@ -2225,13 +2226,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D49">
         <v>133.79</v>
@@ -2245,13 +2246,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D50">
         <v>37.130000000000003</v>
@@ -2265,13 +2266,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D51">
         <v>43.33</v>
@@ -2285,13 +2286,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D52">
         <v>3145.17</v>
@@ -2305,13 +2306,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D53">
         <v>3073.22</v>
@@ -2325,13 +2326,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D54">
         <v>489.6</v>
@@ -2345,13 +2346,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D55">
         <v>926.98</v>
@@ -2365,13 +2366,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D56">
         <v>156.53</v>
@@ -2385,13 +2386,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D57">
         <v>164.15</v>
@@ -2405,13 +2406,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D58">
         <v>482.38</v>
@@ -2424,14 +2425,14 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>126</v>
+      <c r="A59" t="s">
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D59">
         <v>198.84</v>
@@ -2445,13 +2446,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D60">
         <v>185.21</v>
@@ -2465,13 +2466,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D61">
         <v>190.71</v>

</xml_diff>